<commit_message>
Fix panic movement: NPE at get path
</commit_message>
<xml_diff>
--- a/ee/test/JSON Generator.xlsx
+++ b/ee/test/JSON Generator.xlsx
@@ -499,7 +499,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,17 +556,17 @@
       </c>
       <c r="C2">
         <f ca="1">RAND()*1000</f>
-        <v>844.72605042539044</v>
+        <v>52.346769691384409</v>
       </c>
       <c r="J2">
-        <v>9410</v>
+        <v>10081.5026666667</v>
       </c>
       <c r="K2">
-        <v>9560</v>
+        <v>9189.6229999999996</v>
       </c>
       <c r="N2" t="str">
         <f ca="1">CONCATENATE("""",A2,""" :{ ""type"" : """,B2,""", ""event_range"" : ",C2,", ""location"" : { ""x"" : ",J2,", ""y"" : ",K2,"} },")</f>
-        <v>"St. Johannisstift Ev. Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 844.72605042539, "location" : { "x" : 9410, "y" : 9560} },</v>
+        <v>"St. Johannisstift Ev. Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 52.3467696913844, "location" : { "x" : 10081.5026666667, "y" : 9189.623} },</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -578,17 +578,17 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C5" ca="1" si="0">RAND()*1000</f>
-        <v>863.06571513131382</v>
+        <v>697.43450175913244</v>
       </c>
       <c r="J3">
-        <v>11700</v>
+        <v>11039.6716666667</v>
       </c>
       <c r="K3">
-        <v>8560</v>
+        <v>8607.7846666666701</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N4" ca="1" si="1">CONCATENATE("""",A3,""" :{ ""type"" : """,B3,""", ""event_range"" : ",C3,", ""location"" : { ""x"" : ",J3,", ""y"" : ",K3,"} },")</f>
-        <v>"St. Vincenz-Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 863.065715131314, "location" : { "x" : 11700, "y" : 8560} },</v>
+        <v>"St. Vincenz-Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 697.434501759132, "location" : { "x" : 11039.6716666667, "y" : 8607.78466666667} },</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -600,17 +600,17 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>645.55348076132896</v>
+        <v>657.6914784375798</v>
       </c>
       <c r="J4">
-        <v>11600</v>
+        <v>11031.691000000001</v>
       </c>
       <c r="K4">
-        <v>6475</v>
+        <v>7806.0895</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>"Brüderkrankenhaus Sankt Josef" :{ "type" : "HOSPITAL", "event_range" : 645.553480761329, "location" : { "x" : 11600, "y" : 6475} },</v>
+        <v>"Brüderkrankenhaus Sankt Josef" :{ "type" : "HOSPITAL", "event_range" : 657.69147843758, "location" : { "x" : 11031.691, "y" : 7806.0895} },</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -622,17 +622,17 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>825.4769813279579</v>
+        <v>77.9391861174703</v>
       </c>
       <c r="J5">
-        <v>12390</v>
+        <v>11289.561090909099</v>
       </c>
       <c r="K5">
-        <v>4025</v>
+        <v>7600.1217272727299</v>
       </c>
       <c r="N5" t="str">
         <f ca="1">CONCATENATE("""",A5,""" :{ ""type"" : """,B5,""", ""event_range"" : ",C5,", ""location"" : { ""x"" : ",J5,", ""y"" : ",K5,"} },")</f>
-        <v>"Frauen- und Kinderklinik St. Louise" :{ "type" : "HOSPITAL", "event_range" : 825.476981327958, "location" : { "x" : 12390, "y" : 4025} },</v>
+        <v>"Frauen- und Kinderklinik St. Louise" :{ "type" : "HOSPITAL", "event_range" : 77.9391861174703, "location" : { "x" : 11289.5610909091, "y" : 7600.12172727273} },</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -644,43 +644,43 @@
       </c>
       <c r="C6">
         <f ca="1">RAND()*F6*300</f>
-        <v>2336.9234366874266</v>
+        <v>2076.9899925530704</v>
       </c>
       <c r="D6">
         <f ca="1">2*C6</f>
-        <v>4673.8468733748532</v>
+        <v>4153.9799851061407</v>
       </c>
       <c r="E6">
         <f ca="1">C6*3</f>
-        <v>7010.7703100622803</v>
+        <v>6230.9699776592115</v>
       </c>
       <c r="F6">
         <f ca="1">ROUNDUP(10-RAND()*10,0)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6">
         <f ca="1">RANDBETWEEN(0,20000)</f>
-        <v>6777</v>
+        <v>10041</v>
       </c>
       <c r="H6">
-        <f ca="1">RANDBETWEEN(20000,59000)</f>
-        <v>48595</v>
+        <f ca="1">RANDBETWEEN(2000,5900)</f>
+        <v>2699</v>
       </c>
       <c r="I6">
         <f ca="1">G6+H6</f>
-        <v>55372</v>
+        <v>12740</v>
       </c>
       <c r="J6">
         <f ca="1">RANDBETWEEN(0,22000)</f>
-        <v>5879</v>
+        <v>15579</v>
       </c>
       <c r="K6">
         <f ca="1">RANDBETWEEN(0,20000)</f>
-        <v>13070</v>
+        <v>16803</v>
       </c>
       <c r="N6" t="str">
         <f ca="1">CONCATENATE("""",A6,""" :{ ""type"" : """,B6,""", ""event_range"" : ",C6,", ""safe_range"" : ",D6,", ""max_range"" : ",E6,", ""intensity"" : ",F6,", ""start"" : ",G6,", ""end"" : ",I6,", ""location"" : { ""x"" : ",J6,", ""y"" : ",K6,"} },")</f>
-        <v>"event1" :{ "type" : "DISASTER", "event_range" : 2336.92343668743, "safe_range" : 4673.84687337485, "max_range" : 7010.77031006228, "intensity" : 10, "start" : 6777, "end" : 55372, "location" : { "x" : 5879, "y" : 13070} },</v>
+        <v>"event1" :{ "type" : "DISASTER", "event_range" : 2076.98999255307, "safe_range" : 4153.97998510614, "max_range" : 6230.96997765921, "intensity" : 9, "start" : 10041, "end" : 12740, "location" : { "x" : 15579, "y" : 16803} },</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -692,43 +692,43 @@
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C25" ca="1" si="2">RAND()*F7*300</f>
-        <v>1425.2684230746281</v>
+        <v>361.14050007830633</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D25" ca="1" si="3">2*C7</f>
-        <v>2850.5368461492562</v>
+        <v>722.28100015661266</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E25" ca="1" si="4">C7*3</f>
-        <v>4275.8052692238844</v>
+        <v>1083.421500234919</v>
       </c>
       <c r="F7">
         <f t="shared" ref="F7:F25" ca="1" si="5">ROUNDUP(10-RAND()*10,0)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G25" ca="1" si="6">RANDBETWEEN(0,20000)</f>
-        <v>15199</v>
+        <v>5386</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:H25" ca="1" si="7">RANDBETWEEN(20000,59000)</f>
-        <v>54740</v>
+        <f t="shared" ref="H7:H25" ca="1" si="7">RANDBETWEEN(2000,5900)</f>
+        <v>3900</v>
       </c>
       <c r="I7">
         <f t="shared" ref="I7:I25" ca="1" si="8">G7+H7</f>
-        <v>69939</v>
+        <v>9286</v>
       </c>
       <c r="J7">
         <f t="shared" ref="J7:J25" ca="1" si="9">RANDBETWEEN(0,22000)</f>
-        <v>14894</v>
+        <v>14888</v>
       </c>
       <c r="K7">
         <f t="shared" ref="K7:K25" ca="1" si="10">RANDBETWEEN(0,20000)</f>
-        <v>5239</v>
+        <v>4048</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" ref="N7:N24" ca="1" si="11">CONCATENATE("""",A7,""" :{ ""type"" : """,B7,""", ""event_range"" : ",C7,", ""safe_range"" : ",D7,", ""max_range"" : ",E7,", ""intensity"" : ",F7,", ""start"" : ",G7,", ""end"" : ",I7,", ""location"" : { ""x"" : ",J7,", ""y"" : ",K7,"} },")</f>
-        <v>"event2" :{ "type" : "DISASTER", "event_range" : 1425.26842307463, "safe_range" : 2850.53684614926, "max_range" : 4275.80526922388, "intensity" : 5, "start" : 15199, "end" : 69939, "location" : { "x" : 14894, "y" : 5239} },</v>
+        <v>"event2" :{ "type" : "DISASTER", "event_range" : 361.140500078306, "safe_range" : 722.281000156613, "max_range" : 1083.42150023492, "intensity" : 2, "start" : 5386, "end" : 9286, "location" : { "x" : 14888, "y" : 4048} },</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -740,43 +740,43 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="2"/>
-        <v>173.2278400814088</v>
+        <v>2077.1634377409473</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>346.4556801628176</v>
+        <v>4154.3268754818946</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="4"/>
-        <v>519.68352024422643</v>
+        <v>6231.4903132228419</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="6"/>
-        <v>8812</v>
+        <v>14557</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="7"/>
-        <v>53909</v>
+        <v>5679</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="8"/>
-        <v>62721</v>
+        <v>20236</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="9"/>
-        <v>9052</v>
+        <v>4318</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="10"/>
-        <v>5466</v>
+        <v>15832</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event3" :{ "type" : "DISASTER", "event_range" : 173.227840081409, "safe_range" : 346.455680162818, "max_range" : 519.683520244226, "intensity" : 6, "start" : 8812, "end" : 62721, "location" : { "x" : 9052, "y" : 5466} },</v>
+        <v>"event3" :{ "type" : "DISASTER", "event_range" : 2077.16343774095, "safe_range" : 4154.32687548189, "max_range" : 6231.49031322284, "intensity" : 9, "start" : 14557, "end" : 20236, "location" : { "x" : 4318, "y" : 15832} },</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -788,15 +788,15 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="2"/>
-        <v>1298.4214312735198</v>
+        <v>2139.2610365047408</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>2596.8428625470397</v>
+        <v>4278.5220730094816</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="4"/>
-        <v>3895.2642938205595</v>
+        <v>6417.7831095142228</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="5"/>
@@ -804,27 +804,27 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="6"/>
-        <v>16683</v>
+        <v>5222</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="7"/>
-        <v>38423</v>
+        <v>5462</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="8"/>
-        <v>55106</v>
+        <v>10684</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="9"/>
-        <v>17332</v>
+        <v>9023</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="10"/>
-        <v>805</v>
+        <v>3201</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event4" :{ "type" : "DISASTER", "event_range" : 1298.42143127352, "safe_range" : 2596.84286254704, "max_range" : 3895.26429382056, "intensity" : 8, "start" : 16683, "end" : 55106, "location" : { "x" : 17332, "y" : 805} },</v>
+        <v>"event4" :{ "type" : "DISASTER", "event_range" : 2139.26103650474, "safe_range" : 4278.52207300948, "max_range" : 6417.78310951422, "intensity" : 8, "start" : 5222, "end" : 10684, "location" : { "x" : 9023, "y" : 3201} },</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -836,43 +836,43 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="2"/>
-        <v>454.38219920982073</v>
+        <v>2181.9420907609938</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="3"/>
-        <v>908.76439841964145</v>
+        <v>4363.8841815219876</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="4"/>
-        <v>1363.1465976294621</v>
+        <v>6545.8262722829813</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="6"/>
-        <v>13131</v>
+        <v>14962</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="7"/>
-        <v>27134</v>
+        <v>3405</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="8"/>
-        <v>40265</v>
+        <v>18367</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="9"/>
-        <v>21812</v>
+        <v>21167</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="10"/>
-        <v>9399</v>
+        <v>18618</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event5" :{ "type" : "DISASTER", "event_range" : 454.382199209821, "safe_range" : 908.764398419641, "max_range" : 1363.14659762946, "intensity" : 5, "start" : 13131, "end" : 40265, "location" : { "x" : 21812, "y" : 9399} },</v>
+        <v>"event5" :{ "type" : "DISASTER", "event_range" : 2181.94209076099, "safe_range" : 4363.88418152199, "max_range" : 6545.82627228298, "intensity" : 10, "start" : 14962, "end" : 18367, "location" : { "x" : 21167, "y" : 18618} },</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -884,43 +884,43 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="2"/>
-        <v>50.375800981258436</v>
+        <v>279.57922992842316</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="3"/>
-        <v>100.75160196251687</v>
+        <v>559.15845985684632</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="4"/>
-        <v>151.12740294377531</v>
+        <v>838.73768978526948</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="6"/>
-        <v>2962</v>
+        <v>12732</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="7"/>
-        <v>32064</v>
+        <v>4049</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="8"/>
-        <v>35026</v>
+        <v>16781</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="9"/>
-        <v>957</v>
+        <v>6938</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="10"/>
-        <v>10898</v>
+        <v>4895</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event6" :{ "type" : "DISASTER", "event_range" : 50.3758009812584, "safe_range" : 100.751601962517, "max_range" : 151.127402943775, "intensity" : 5, "start" : 2962, "end" : 35026, "location" : { "x" : 957, "y" : 10898} },</v>
+        <v>"event6" :{ "type" : "DISASTER", "event_range" : 279.579229928423, "safe_range" : 559.158459856846, "max_range" : 838.737689785269, "intensity" : 3, "start" : 12732, "end" : 16781, "location" : { "x" : 6938, "y" : 4895} },</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -932,43 +932,43 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="2"/>
-        <v>459.74797048154767</v>
+        <v>1117.7135748753583</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="3"/>
-        <v>919.49594096309534</v>
+        <v>2235.4271497507166</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="4"/>
-        <v>1379.2439114446429</v>
+        <v>3353.1407246260751</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="6"/>
-        <v>17830</v>
+        <v>11218</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="7"/>
-        <v>31612</v>
+        <v>3169</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="8"/>
-        <v>49442</v>
+        <v>14387</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="9"/>
-        <v>21955</v>
+        <v>2151</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="10"/>
-        <v>9540</v>
+        <v>1930</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event7" :{ "type" : "DISASTER", "event_range" : 459.747970481548, "safe_range" : 919.495940963095, "max_range" : 1379.24391144464, "intensity" : 2, "start" : 17830, "end" : 49442, "location" : { "x" : 21955, "y" : 9540} },</v>
+        <v>"event7" :{ "type" : "DISASTER", "event_range" : 1117.71357487536, "safe_range" : 2235.42714975072, "max_range" : 3353.14072462608, "intensity" : 7, "start" : 11218, "end" : 14387, "location" : { "x" : 2151, "y" : 1930} },</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -980,43 +980,43 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="2"/>
-        <v>68.226215051952764</v>
+        <v>1503.0016816284181</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="3"/>
-        <v>136.45243010390553</v>
+        <v>3006.0033632568361</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="4"/>
-        <v>204.67864515585831</v>
+        <v>4509.0050448852544</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="6"/>
-        <v>13581</v>
+        <v>19786</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="7"/>
-        <v>32646</v>
+        <v>2940</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="8"/>
-        <v>46227</v>
+        <v>22726</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="9"/>
-        <v>10703</v>
+        <v>21422</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="10"/>
-        <v>6150</v>
+        <v>19251</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event8" :{ "type" : "DISASTER", "event_range" : 68.2262150519528, "safe_range" : 136.452430103906, "max_range" : 204.678645155858, "intensity" : 6, "start" : 13581, "end" : 46227, "location" : { "x" : 10703, "y" : 6150} },</v>
+        <v>"event8" :{ "type" : "DISASTER", "event_range" : 1503.00168162842, "safe_range" : 3006.00336325684, "max_range" : 4509.00504488525, "intensity" : 7, "start" : 19786, "end" : 22726, "location" : { "x" : 21422, "y" : 19251} },</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1028,43 +1028,43 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="2"/>
-        <v>2307.5841865485982</v>
+        <v>1339.4859530221479</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="3"/>
-        <v>4615.1683730971963</v>
+        <v>2678.9719060442958</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="4"/>
-        <v>6922.7525596457945</v>
+        <v>4018.4578590664437</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="6"/>
-        <v>17652</v>
+        <v>11422</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="7"/>
-        <v>31931</v>
+        <v>4032</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="8"/>
-        <v>49583</v>
+        <v>15454</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="9"/>
-        <v>20248</v>
+        <v>18609</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="10"/>
-        <v>13883</v>
+        <v>3328</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event9" :{ "type" : "DISASTER", "event_range" : 2307.5841865486, "safe_range" : 4615.1683730972, "max_range" : 6922.75255964579, "intensity" : 9, "start" : 17652, "end" : 49583, "location" : { "x" : 20248, "y" : 13883} },</v>
+        <v>"event9" :{ "type" : "DISASTER", "event_range" : 1339.48595302215, "safe_range" : 2678.9719060443, "max_range" : 4018.45785906644, "intensity" : 6, "start" : 11422, "end" : 15454, "location" : { "x" : 18609, "y" : 3328} },</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1076,43 +1076,43 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="2"/>
-        <v>1581.7886017806566</v>
+        <v>265.23878803823175</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="3"/>
-        <v>3163.5772035613131</v>
+        <v>530.47757607646349</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="4"/>
-        <v>4745.3658053419695</v>
+        <v>795.71636411469524</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="6"/>
-        <v>5566</v>
+        <v>19794</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="7"/>
-        <v>51014</v>
+        <v>5034</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="8"/>
-        <v>56580</v>
+        <v>24828</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="9"/>
-        <v>14066</v>
+        <v>2580</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="10"/>
-        <v>1698</v>
+        <v>13380</v>
       </c>
       <c r="N15" t="str">
-        <f ca="1">CONCATENATE("""",A15,""" :{ ""type"" : """,B15,""", ""event_range"" : ",C15,", ""safe_range"" : ",D15,", ""max_range"" : ",E15,", ""intensity"" : ",F15,", ""start"" : ",G15,", ""end"" : ",I15,", ""location"" : { ""x"" : I13",J15,", ""y"" : ",K15,"} },")</f>
-        <v>"event10" :{ "type" : "DISASTER", "event_range" : 1581.78860178066, "safe_range" : 3163.57720356131, "max_range" : 4745.36580534197, "intensity" : 9, "start" : 5566, "end" : 56580, "location" : { "x" : I1314066, "y" : 1698} },</v>
+        <f ca="1">CONCATENATE("""",A15,""" :{ ""type"" : """,B15,""", ""event_range"" : ",C15,", ""safe_range"" : ",D15,", ""max_range"" : ",E15,", ""intensity"" : ",F15,", ""start"" : ",G15,", ""end"" : ",I15,", ""location"" : { ""x"" : ",J15,", ""y"" : ",K15,"} },")</f>
+        <v>"event10" :{ "type" : "DISASTER", "event_range" : 265.238788038232, "safe_range" : 530.477576076463, "max_range" : 795.716364114695, "intensity" : 1, "start" : 19794, "end" : 24828, "location" : { "x" : 2580, "y" : 13380} },</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1124,43 +1124,43 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="2"/>
-        <v>261.76607170458431</v>
+        <v>2252.5284548258028</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="3"/>
-        <v>523.53214340916861</v>
+        <v>4505.0569096516056</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="4"/>
-        <v>785.29821511375292</v>
+        <v>6757.5853644774088</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="6"/>
-        <v>4383</v>
+        <v>6269</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="7"/>
-        <v>57701</v>
+        <v>5400</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="8"/>
-        <v>62084</v>
+        <v>11669</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="9"/>
-        <v>1221</v>
+        <v>5447</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="10"/>
-        <v>5648</v>
+        <v>16928</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event11" :{ "type" : "DISASTER", "event_range" : 261.766071704584, "safe_range" : 523.532143409169, "max_range" : 785.298215113753, "intensity" : 6, "start" : 4383, "end" : 62084, "location" : { "x" : 1221, "y" : 5648} },</v>
+        <v>"event11" :{ "type" : "DISASTER", "event_range" : 2252.5284548258, "safe_range" : 4505.05690965161, "max_range" : 6757.58536447741, "intensity" : 8, "start" : 6269, "end" : 11669, "location" : { "x" : 5447, "y" : 16928} },</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1172,43 +1172,43 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="2"/>
-        <v>496.1003518765076</v>
+        <v>266.31532961920425</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="3"/>
-        <v>992.2007037530152</v>
+        <v>532.6306592384085</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="4"/>
-        <v>1488.3010556295228</v>
+        <v>798.94598885761275</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="6"/>
-        <v>6316</v>
+        <v>16554</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="7"/>
-        <v>45334</v>
+        <v>5353</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="8"/>
-        <v>51650</v>
+        <v>21907</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="9"/>
-        <v>10525</v>
+        <v>11439</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="10"/>
-        <v>16872</v>
+        <v>8804</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event12" :{ "type" : "DISASTER", "event_range" : 496.100351876508, "safe_range" : 992.200703753015, "max_range" : 1488.30105562952, "intensity" : 2, "start" : 6316, "end" : 51650, "location" : { "x" : 10525, "y" : 16872} },</v>
+        <v>"event12" :{ "type" : "DISASTER", "event_range" : 266.315329619204, "safe_range" : 532.630659238408, "max_range" : 798.945988857613, "intensity" : 1, "start" : 16554, "end" : 21907, "location" : { "x" : 11439, "y" : 8804} },</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1220,43 +1220,43 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="2"/>
-        <v>1008.0272780581211</v>
+        <v>717.81028048813937</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="3"/>
-        <v>2016.0545561162421</v>
+        <v>1435.6205609762787</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="4"/>
-        <v>3024.0818341743634</v>
+        <v>2153.4308414644183</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="6"/>
-        <v>16017</v>
+        <v>19467</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="7"/>
-        <v>24199</v>
+        <v>5202</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="8"/>
-        <v>40216</v>
+        <v>24669</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="9"/>
-        <v>6986</v>
+        <v>13681</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="10"/>
-        <v>13004</v>
+        <v>15790</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event13" :{ "type" : "DISASTER", "event_range" : 1008.02727805812, "safe_range" : 2016.05455611624, "max_range" : 3024.08183417436, "intensity" : 4, "start" : 16017, "end" : 40216, "location" : { "x" : 6986, "y" : 13004} },</v>
+        <v>"event13" :{ "type" : "DISASTER", "event_range" : 717.810280488139, "safe_range" : 1435.62056097628, "max_range" : 2153.43084146442, "intensity" : 9, "start" : 19467, "end" : 24669, "location" : { "x" : 13681, "y" : 15790} },</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1268,43 +1268,43 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2010117990530782</v>
+        <v>202.06882537468653</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="3"/>
-        <v>8.4020235981061564</v>
+        <v>404.13765074937305</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="4"/>
-        <v>12.603035397159235</v>
+        <v>606.20647612405958</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="6"/>
-        <v>4212</v>
+        <v>4772</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="7"/>
-        <v>43406</v>
+        <v>2610</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="8"/>
-        <v>47618</v>
+        <v>7382</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="9"/>
-        <v>4777</v>
+        <v>12929</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="10"/>
-        <v>9846</v>
+        <v>15329</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event14" :{ "type" : "DISASTER", "event_range" : 4.20101179905308, "safe_range" : 8.40202359810616, "max_range" : 12.6030353971592, "intensity" : 10, "start" : 4212, "end" : 47618, "location" : { "x" : 4777, "y" : 9846} },</v>
+        <v>"event14" :{ "type" : "DISASTER", "event_range" : 202.068825374687, "safe_range" : 404.137650749373, "max_range" : 606.20647612406, "intensity" : 4, "start" : 4772, "end" : 7382, "location" : { "x" : 12929, "y" : 15329} },</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1316,43 +1316,43 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="2"/>
-        <v>345.6943305724983</v>
+        <v>469.16188687167823</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="3"/>
-        <v>691.3886611449966</v>
+        <v>938.32377374335647</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="4"/>
-        <v>1037.0829917174949</v>
+        <v>1407.4856606150347</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="6"/>
-        <v>12036</v>
+        <v>6033</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="7"/>
-        <v>31272</v>
+        <v>2611</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="8"/>
-        <v>43308</v>
+        <v>8644</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="9"/>
-        <v>19386</v>
+        <v>19937</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="10"/>
-        <v>18794</v>
+        <v>10045</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event15" :{ "type" : "DISASTER", "event_range" : 345.694330572498, "safe_range" : 691.388661144997, "max_range" : 1037.08299171749, "intensity" : 9, "start" : 12036, "end" : 43308, "location" : { "x" : 19386, "y" : 18794} },</v>
+        <v>"event15" :{ "type" : "DISASTER", "event_range" : 469.161886871678, "safe_range" : 938.323773743356, "max_range" : 1407.48566061503, "intensity" : 10, "start" : 6033, "end" : 8644, "location" : { "x" : 19937, "y" : 10045} },</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1364,43 +1364,43 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="2"/>
-        <v>2061.362526608727</v>
+        <v>1204.0297562938065</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="3"/>
-        <v>4122.7250532174539</v>
+        <v>2408.059512587613</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="4"/>
-        <v>6184.0875798261804</v>
+        <v>3612.0892688814192</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="6"/>
-        <v>10287</v>
+        <v>7225</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="7"/>
-        <v>36893</v>
+        <v>2068</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="8"/>
-        <v>47180</v>
+        <v>9293</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="9"/>
-        <v>12085</v>
+        <v>11652</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="10"/>
-        <v>3025</v>
+        <v>13493</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event16" :{ "type" : "DISASTER", "event_range" : 2061.36252660873, "safe_range" : 4122.72505321745, "max_range" : 6184.08757982618, "intensity" : 9, "start" : 10287, "end" : 47180, "location" : { "x" : 12085, "y" : 3025} },</v>
+        <v>"event16" :{ "type" : "DISASTER", "event_range" : 1204.02975629381, "safe_range" : 2408.05951258761, "max_range" : 3612.08926888142, "intensity" : 6, "start" : 7225, "end" : 9293, "location" : { "x" : 11652, "y" : 13493} },</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1412,43 +1412,43 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="2"/>
-        <v>1727.5864958685293</v>
+        <v>601.03672248573662</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="3"/>
-        <v>3455.1729917370585</v>
+        <v>1202.0734449714732</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="4"/>
-        <v>5182.7594876055882</v>
+        <v>1803.1101674572099</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="6"/>
-        <v>7129</v>
+        <v>4413</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="7"/>
-        <v>38777</v>
+        <v>2695</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="8"/>
-        <v>45906</v>
+        <v>7108</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="9"/>
-        <v>4848</v>
+        <v>21100</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="10"/>
-        <v>12543</v>
+        <v>14927</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event17" :{ "type" : "DISASTER", "event_range" : 1727.58649586853, "safe_range" : 3455.17299173706, "max_range" : 5182.75948760559, "intensity" : 10, "start" : 7129, "end" : 45906, "location" : { "x" : 4848, "y" : 12543} },</v>
+        <v>"event17" :{ "type" : "DISASTER", "event_range" : 601.036722485737, "safe_range" : 1202.07344497147, "max_range" : 1803.11016745721, "intensity" : 4, "start" : 4413, "end" : 7108, "location" : { "x" : 21100, "y" : 14927} },</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1460,43 +1460,43 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="2"/>
-        <v>232.98263496675045</v>
+        <v>340.06742970834853</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="3"/>
-        <v>465.96526993350091</v>
+        <v>680.13485941669705</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="4"/>
-        <v>698.94790490025139</v>
+        <v>1020.2022891250456</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="6"/>
-        <v>3024</v>
+        <v>17217</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="7"/>
-        <v>37599</v>
+        <v>3068</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="8"/>
-        <v>40623</v>
+        <v>20285</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="9"/>
-        <v>19395</v>
+        <v>10910</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="10"/>
-        <v>3060</v>
+        <v>4409</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event18" :{ "type" : "DISASTER", "event_range" : 232.98263496675, "safe_range" : 465.965269933501, "max_range" : 698.947904900251, "intensity" : 1, "start" : 3024, "end" : 40623, "location" : { "x" : 19395, "y" : 3060} },</v>
+        <v>"event18" :{ "type" : "DISASTER", "event_range" : 340.067429708349, "safe_range" : 680.134859416697, "max_range" : 1020.20228912505, "intensity" : 3, "start" : 17217, "end" : 20285, "location" : { "x" : 10910, "y" : 4409} },</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1508,43 +1508,43 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="2"/>
-        <v>1685.5513916682273</v>
+        <v>227.54643708175388</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="3"/>
-        <v>3371.1027833364546</v>
+        <v>455.09287416350776</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="4"/>
-        <v>5056.6541750046817</v>
+        <v>682.63931124526164</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="6"/>
-        <v>5552</v>
+        <v>12179</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="7"/>
-        <v>30392</v>
+        <v>4846</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="8"/>
-        <v>35944</v>
+        <v>17025</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="9"/>
-        <v>10093</v>
+        <v>5367</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="10"/>
-        <v>3346</v>
+        <v>7293</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event19" :{ "type" : "DISASTER", "event_range" : 1685.55139166823, "safe_range" : 3371.10278333645, "max_range" : 5056.65417500468, "intensity" : 8, "start" : 5552, "end" : 35944, "location" : { "x" : 10093, "y" : 3346} },</v>
+        <v>"event19" :{ "type" : "DISASTER", "event_range" : 227.546437081754, "safe_range" : 455.092874163508, "max_range" : 682.639311245262, "intensity" : 2, "start" : 12179, "end" : 17025, "location" : { "x" : 5367, "y" : 7293} },</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1556,43 +1556,43 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="2"/>
-        <v>538.80554729133621</v>
+        <v>276.38597663590355</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="3"/>
-        <v>1077.6110945826724</v>
+        <v>552.77195327180709</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="4"/>
-        <v>1616.4166418740087</v>
+        <v>829.1579299077107</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="6"/>
-        <v>14382</v>
+        <v>4104</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="7"/>
-        <v>30828</v>
+        <v>3738</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="8"/>
-        <v>45210</v>
+        <v>7842</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="9"/>
-        <v>19763</v>
+        <v>5997</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="10"/>
-        <v>18493</v>
+        <v>14536</v>
       </c>
       <c r="N25" t="str">
         <f ca="1">CONCATENATE("""",A25,""" :{ ""type"" : """,B25,""", ""event_range"" : ",C25,", ""safe_range"" : ",D25,", ""max_range"" : ",E25,", ""intensity"" : ",F25,", ""start"" : ",G25,", ""end"" : ",I25,", ""location"" : { ""x"" : ",J25,", ""y"" : ",K25,"} }")</f>
-        <v>"event20" :{ "type" : "DISASTER", "event_range" : 538.805547291336, "safe_range" : 1077.61109458267, "max_range" : 1616.41664187401, "intensity" : 2, "start" : 14382, "end" : 45210, "location" : { "x" : 19763, "y" : 18493} }</v>
+        <v>"event20" :{ "type" : "DISASTER", "event_range" : 276.385976635904, "safe_range" : 552.771953271807, "max_range" : 829.157929907711, "intensity" : 3, "start" : 4104, "end" : 7842, "location" : { "x" : 5997, "y" : 14536} }</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correct the hospital's position in VHMTestFast
</commit_message>
<xml_diff>
--- a/ee/test/JSON Generator.xlsx
+++ b/ee/test/JSON Generator.xlsx
@@ -499,7 +499,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,17 +556,17 @@
       </c>
       <c r="C2">
         <f ca="1">RAND()*1000</f>
-        <v>52.346769691384409</v>
+        <v>117.34916185302747</v>
       </c>
       <c r="J2">
-        <v>10081.5026666667</v>
+        <v>10173.82</v>
       </c>
       <c r="K2">
-        <v>9189.6229999999996</v>
+        <v>10612.26</v>
       </c>
       <c r="N2" t="str">
         <f ca="1">CONCATENATE("""",A2,""" :{ ""type"" : """,B2,""", ""event_range"" : ",C2,", ""location"" : { ""x"" : ",J2,", ""y"" : ",K2,"} },")</f>
-        <v>"St. Johannisstift Ev. Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 52.3467696913844, "location" : { "x" : 10081.5026666667, "y" : 9189.623} },</v>
+        <v>"St. Johannisstift Ev. Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 117.349161853027, "location" : { "x" : 10173.82, "y" : 10612.26} },</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -578,17 +578,17 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C5" ca="1" si="0">RAND()*1000</f>
-        <v>697.43450175913244</v>
+        <v>254.99026873700183</v>
       </c>
       <c r="J3">
-        <v>11039.6716666667</v>
+        <v>10928.49</v>
       </c>
       <c r="K3">
-        <v>8607.7846666666701</v>
+        <v>11053.11</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N4" ca="1" si="1">CONCATENATE("""",A3,""" :{ ""type"" : """,B3,""", ""event_range"" : ",C3,", ""location"" : { ""x"" : ",J3,", ""y"" : ",K3,"} },")</f>
-        <v>"St. Vincenz-Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 697.434501759132, "location" : { "x" : 11039.6716666667, "y" : 8607.78466666667} },</v>
+        <v>"St. Vincenz-Krankenhaus" :{ "type" : "HOSPITAL", "event_range" : 254.990268737002, "location" : { "x" : 10928.49, "y" : 11053.11} },</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -600,17 +600,17 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>657.6914784375798</v>
+        <v>321.14824409919328</v>
       </c>
       <c r="J4">
-        <v>11031.691000000001</v>
+        <v>11035.67</v>
       </c>
       <c r="K4">
-        <v>7806.0895</v>
+        <v>11862.38</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>"Brüderkrankenhaus Sankt Josef" :{ "type" : "HOSPITAL", "event_range" : 657.69147843758, "location" : { "x" : 11031.691, "y" : 7806.0895} },</v>
+        <v>"Brüderkrankenhaus Sankt Josef" :{ "type" : "HOSPITAL", "event_range" : 321.148244099193, "location" : { "x" : 11035.67, "y" : 11862.38} },</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -622,17 +622,17 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>77.9391861174703</v>
+        <v>703.75004306078972</v>
       </c>
       <c r="J5">
-        <v>11289.561090909099</v>
+        <v>11236.37</v>
       </c>
       <c r="K5">
-        <v>7600.1217272727299</v>
+        <v>12208.07</v>
       </c>
       <c r="N5" t="str">
         <f ca="1">CONCATENATE("""",A5,""" :{ ""type"" : """,B5,""", ""event_range"" : ",C5,", ""location"" : { ""x"" : ",J5,", ""y"" : ",K5,"} },")</f>
-        <v>"Frauen- und Kinderklinik St. Louise" :{ "type" : "HOSPITAL", "event_range" : 77.9391861174703, "location" : { "x" : 11289.5610909091, "y" : 7600.12172727273} },</v>
+        <v>"Frauen- und Kinderklinik St. Louise" :{ "type" : "HOSPITAL", "event_range" : 703.75004306079, "location" : { "x" : 11236.37, "y" : 12208.07} },</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -644,43 +644,43 @@
       </c>
       <c r="C6">
         <f ca="1">RAND()*F6*300</f>
-        <v>2076.9899925530704</v>
+        <v>1241.6810361412759</v>
       </c>
       <c r="D6">
         <f ca="1">2*C6</f>
-        <v>4153.9799851061407</v>
+        <v>2483.3620722825517</v>
       </c>
       <c r="E6">
         <f ca="1">C6*3</f>
-        <v>6230.9699776592115</v>
+        <v>3725.0431084238276</v>
       </c>
       <c r="F6">
         <f ca="1">ROUNDUP(10-RAND()*10,0)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <f ca="1">RANDBETWEEN(0,20000)</f>
-        <v>10041</v>
+        <v>987</v>
       </c>
       <c r="H6">
         <f ca="1">RANDBETWEEN(2000,5900)</f>
-        <v>2699</v>
+        <v>5790</v>
       </c>
       <c r="I6">
         <f ca="1">G6+H6</f>
-        <v>12740</v>
+        <v>6777</v>
       </c>
       <c r="J6">
         <f ca="1">RANDBETWEEN(0,22000)</f>
-        <v>15579</v>
+        <v>21640</v>
       </c>
       <c r="K6">
         <f ca="1">RANDBETWEEN(0,20000)</f>
-        <v>16803</v>
+        <v>10570</v>
       </c>
       <c r="N6" t="str">
         <f ca="1">CONCATENATE("""",A6,""" :{ ""type"" : """,B6,""", ""event_range"" : ",C6,", ""safe_range"" : ",D6,", ""max_range"" : ",E6,", ""intensity"" : ",F6,", ""start"" : ",G6,", ""end"" : ",I6,", ""location"" : { ""x"" : ",J6,", ""y"" : ",K6,"} },")</f>
-        <v>"event1" :{ "type" : "DISASTER", "event_range" : 2076.98999255307, "safe_range" : 4153.97998510614, "max_range" : 6230.96997765921, "intensity" : 9, "start" : 10041, "end" : 12740, "location" : { "x" : 15579, "y" : 16803} },</v>
+        <v>"event1" :{ "type" : "DISASTER", "event_range" : 1241.68103614128, "safe_range" : 2483.36207228255, "max_range" : 3725.04310842383, "intensity" : 5, "start" : 987, "end" : 6777, "location" : { "x" : 21640, "y" : 10570} },</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -692,43 +692,43 @@
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C25" ca="1" si="2">RAND()*F7*300</f>
-        <v>361.14050007830633</v>
+        <v>740.5649418314963</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D25" ca="1" si="3">2*C7</f>
-        <v>722.28100015661266</v>
+        <v>1481.1298836629926</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E25" ca="1" si="4">C7*3</f>
-        <v>1083.421500234919</v>
+        <v>2221.6948254944891</v>
       </c>
       <c r="F7">
         <f t="shared" ref="F7:F25" ca="1" si="5">ROUNDUP(10-RAND()*10,0)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G25" ca="1" si="6">RANDBETWEEN(0,20000)</f>
-        <v>5386</v>
+        <v>19170</v>
       </c>
       <c r="H7">
         <f t="shared" ref="H7:H25" ca="1" si="7">RANDBETWEEN(2000,5900)</f>
-        <v>3900</v>
+        <v>3325</v>
       </c>
       <c r="I7">
         <f t="shared" ref="I7:I25" ca="1" si="8">G7+H7</f>
-        <v>9286</v>
+        <v>22495</v>
       </c>
       <c r="J7">
         <f t="shared" ref="J7:J25" ca="1" si="9">RANDBETWEEN(0,22000)</f>
-        <v>14888</v>
+        <v>8719</v>
       </c>
       <c r="K7">
         <f t="shared" ref="K7:K25" ca="1" si="10">RANDBETWEEN(0,20000)</f>
-        <v>4048</v>
+        <v>14407</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" ref="N7:N24" ca="1" si="11">CONCATENATE("""",A7,""" :{ ""type"" : """,B7,""", ""event_range"" : ",C7,", ""safe_range"" : ",D7,", ""max_range"" : ",E7,", ""intensity"" : ",F7,", ""start"" : ",G7,", ""end"" : ",I7,", ""location"" : { ""x"" : ",J7,", ""y"" : ",K7,"} },")</f>
-        <v>"event2" :{ "type" : "DISASTER", "event_range" : 361.140500078306, "safe_range" : 722.281000156613, "max_range" : 1083.42150023492, "intensity" : 2, "start" : 5386, "end" : 9286, "location" : { "x" : 14888, "y" : 4048} },</v>
+        <v>"event2" :{ "type" : "DISASTER", "event_range" : 740.564941831496, "safe_range" : 1481.12988366299, "max_range" : 2221.69482549449, "intensity" : 6, "start" : 19170, "end" : 22495, "location" : { "x" : 8719, "y" : 14407} },</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -740,43 +740,43 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="2"/>
-        <v>2077.1634377409473</v>
+        <v>434.83215379870751</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>4154.3268754818946</v>
+        <v>869.66430759741502</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="4"/>
-        <v>6231.4903132228419</v>
+        <v>1304.4964613961224</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="6"/>
-        <v>14557</v>
+        <v>15122</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="7"/>
-        <v>5679</v>
+        <v>2635</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="8"/>
-        <v>20236</v>
+        <v>17757</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="9"/>
-        <v>4318</v>
+        <v>20711</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="10"/>
-        <v>15832</v>
+        <v>12802</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event3" :{ "type" : "DISASTER", "event_range" : 2077.16343774095, "safe_range" : 4154.32687548189, "max_range" : 6231.49031322284, "intensity" : 9, "start" : 14557, "end" : 20236, "location" : { "x" : 4318, "y" : 15832} },</v>
+        <v>"event3" :{ "type" : "DISASTER", "event_range" : 434.832153798708, "safe_range" : 869.664307597415, "max_range" : 1304.49646139612, "intensity" : 5, "start" : 15122, "end" : 17757, "location" : { "x" : 20711, "y" : 12802} },</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -788,43 +788,43 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="2"/>
-        <v>2139.2610365047408</v>
+        <v>756.0562228853837</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>4278.5220730094816</v>
+        <v>1512.1124457707674</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="4"/>
-        <v>6417.7831095142228</v>
+        <v>2268.1686686561511</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="6"/>
-        <v>5222</v>
+        <v>2184</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="7"/>
-        <v>5462</v>
+        <v>3508</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="8"/>
-        <v>10684</v>
+        <v>5692</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="9"/>
-        <v>9023</v>
+        <v>15501</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="10"/>
-        <v>3201</v>
+        <v>18355</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event4" :{ "type" : "DISASTER", "event_range" : 2139.26103650474, "safe_range" : 4278.52207300948, "max_range" : 6417.78310951422, "intensity" : 8, "start" : 5222, "end" : 10684, "location" : { "x" : 9023, "y" : 3201} },</v>
+        <v>"event4" :{ "type" : "DISASTER", "event_range" : 756.056222885384, "safe_range" : 1512.11244577077, "max_range" : 2268.16866865615, "intensity" : 10, "start" : 2184, "end" : 5692, "location" : { "x" : 15501, "y" : 18355} },</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -836,43 +836,43 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="2"/>
-        <v>2181.9420907609938</v>
+        <v>192.65299952550413</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="3"/>
-        <v>4363.8841815219876</v>
+        <v>385.30599905100826</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="4"/>
-        <v>6545.8262722829813</v>
+        <v>577.95899857651239</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="6"/>
-        <v>14962</v>
+        <v>7114</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="7"/>
-        <v>3405</v>
+        <v>5662</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="8"/>
-        <v>18367</v>
+        <v>12776</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="9"/>
-        <v>21167</v>
+        <v>9861</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="10"/>
-        <v>18618</v>
+        <v>3105</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event5" :{ "type" : "DISASTER", "event_range" : 2181.94209076099, "safe_range" : 4363.88418152199, "max_range" : 6545.82627228298, "intensity" : 10, "start" : 14962, "end" : 18367, "location" : { "x" : 21167, "y" : 18618} },</v>
+        <v>"event5" :{ "type" : "DISASTER", "event_range" : 192.652999525504, "safe_range" : 385.305999051008, "max_range" : 577.958998576512, "intensity" : 7, "start" : 7114, "end" : 12776, "location" : { "x" : 9861, "y" : 3105} },</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -884,43 +884,43 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="2"/>
-        <v>279.57922992842316</v>
+        <v>122.43864197387575</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="3"/>
-        <v>559.15845985684632</v>
+        <v>244.87728394775149</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="4"/>
-        <v>838.73768978526948</v>
+        <v>367.31592592162724</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="6"/>
-        <v>12732</v>
+        <v>13202</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="7"/>
-        <v>4049</v>
+        <v>3644</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="8"/>
-        <v>16781</v>
+        <v>16846</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="9"/>
-        <v>6938</v>
+        <v>20510</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="10"/>
-        <v>4895</v>
+        <v>19937</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event6" :{ "type" : "DISASTER", "event_range" : 279.579229928423, "safe_range" : 559.158459856846, "max_range" : 838.737689785269, "intensity" : 3, "start" : 12732, "end" : 16781, "location" : { "x" : 6938, "y" : 4895} },</v>
+        <v>"event6" :{ "type" : "DISASTER", "event_range" : 122.438641973876, "safe_range" : 244.877283947751, "max_range" : 367.315925921627, "intensity" : 2, "start" : 13202, "end" : 16846, "location" : { "x" : 20510, "y" : 19937} },</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -932,43 +932,43 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="2"/>
-        <v>1117.7135748753583</v>
+        <v>898.63698693271908</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="3"/>
-        <v>2235.4271497507166</v>
+        <v>1797.2739738654382</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="4"/>
-        <v>3353.1407246260751</v>
+        <v>2695.9109607981572</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="6"/>
-        <v>11218</v>
+        <v>19167</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="7"/>
-        <v>3169</v>
+        <v>4098</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="8"/>
-        <v>14387</v>
+        <v>23265</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="9"/>
-        <v>2151</v>
+        <v>15895</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="10"/>
-        <v>1930</v>
+        <v>1581</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event7" :{ "type" : "DISASTER", "event_range" : 1117.71357487536, "safe_range" : 2235.42714975072, "max_range" : 3353.14072462608, "intensity" : 7, "start" : 11218, "end" : 14387, "location" : { "x" : 2151, "y" : 1930} },</v>
+        <v>"event7" :{ "type" : "DISASTER", "event_range" : 898.636986932719, "safe_range" : 1797.27397386544, "max_range" : 2695.91096079816, "intensity" : 10, "start" : 19167, "end" : 23265, "location" : { "x" : 15895, "y" : 1581} },</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -980,43 +980,43 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="2"/>
-        <v>1503.0016816284181</v>
+        <v>527.33749379000005</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="3"/>
-        <v>3006.0033632568361</v>
+        <v>1054.6749875800001</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="4"/>
-        <v>4509.0050448852544</v>
+        <v>1582.0124813700002</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="6"/>
-        <v>19786</v>
+        <v>9401</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="7"/>
-        <v>2940</v>
+        <v>2552</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="8"/>
-        <v>22726</v>
+        <v>11953</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="9"/>
-        <v>21422</v>
+        <v>12401</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="10"/>
-        <v>19251</v>
+        <v>5384</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event8" :{ "type" : "DISASTER", "event_range" : 1503.00168162842, "safe_range" : 3006.00336325684, "max_range" : 4509.00504488525, "intensity" : 7, "start" : 19786, "end" : 22726, "location" : { "x" : 21422, "y" : 19251} },</v>
+        <v>"event8" :{ "type" : "DISASTER", "event_range" : 527.33749379, "safe_range" : 1054.67498758, "max_range" : 1582.01248137, "intensity" : 4, "start" : 9401, "end" : 11953, "location" : { "x" : 12401, "y" : 5384} },</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1028,43 +1028,43 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="2"/>
-        <v>1339.4859530221479</v>
+        <v>452.41397376320805</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="3"/>
-        <v>2678.9719060442958</v>
+        <v>904.8279475264161</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="4"/>
-        <v>4018.4578590664437</v>
+        <v>1357.2419212896241</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="6"/>
-        <v>11422</v>
+        <v>12915</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="7"/>
-        <v>4032</v>
+        <v>4872</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="8"/>
-        <v>15454</v>
+        <v>17787</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="9"/>
-        <v>18609</v>
+        <v>11598</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="10"/>
-        <v>3328</v>
+        <v>19498</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event9" :{ "type" : "DISASTER", "event_range" : 1339.48595302215, "safe_range" : 2678.9719060443, "max_range" : 4018.45785906644, "intensity" : 6, "start" : 11422, "end" : 15454, "location" : { "x" : 18609, "y" : 3328} },</v>
+        <v>"event9" :{ "type" : "DISASTER", "event_range" : 452.413973763208, "safe_range" : 904.827947526416, "max_range" : 1357.24192128962, "intensity" : 2, "start" : 12915, "end" : 17787, "location" : { "x" : 11598, "y" : 19498} },</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1076,43 +1076,43 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="2"/>
-        <v>265.23878803823175</v>
+        <v>1300.61762184397</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="3"/>
-        <v>530.47757607646349</v>
+        <v>2601.2352436879401</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="4"/>
-        <v>795.71636411469524</v>
+        <v>3901.8528655319101</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="6"/>
-        <v>19794</v>
+        <v>6470</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="7"/>
-        <v>5034</v>
+        <v>5265</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="8"/>
-        <v>24828</v>
+        <v>11735</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="9"/>
-        <v>2580</v>
+        <v>8931</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="10"/>
-        <v>13380</v>
+        <v>1197</v>
       </c>
       <c r="N15" t="str">
         <f ca="1">CONCATENATE("""",A15,""" :{ ""type"" : """,B15,""", ""event_range"" : ",C15,", ""safe_range"" : ",D15,", ""max_range"" : ",E15,", ""intensity"" : ",F15,", ""start"" : ",G15,", ""end"" : ",I15,", ""location"" : { ""x"" : ",J15,", ""y"" : ",K15,"} },")</f>
-        <v>"event10" :{ "type" : "DISASTER", "event_range" : 265.238788038232, "safe_range" : 530.477576076463, "max_range" : 795.716364114695, "intensity" : 1, "start" : 19794, "end" : 24828, "location" : { "x" : 2580, "y" : 13380} },</v>
+        <v>"event10" :{ "type" : "DISASTER", "event_range" : 1300.61762184397, "safe_range" : 2601.23524368794, "max_range" : 3901.85286553191, "intensity" : 5, "start" : 6470, "end" : 11735, "location" : { "x" : 8931, "y" : 1197} },</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1124,43 +1124,43 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="2"/>
-        <v>2252.5284548258028</v>
+        <v>217.9694890485726</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="3"/>
-        <v>4505.0569096516056</v>
+        <v>435.9389780971452</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="4"/>
-        <v>6757.5853644774088</v>
+        <v>653.90846714571785</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="6"/>
-        <v>6269</v>
+        <v>481</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="7"/>
-        <v>5400</v>
+        <v>3729</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="8"/>
-        <v>11669</v>
+        <v>4210</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="9"/>
-        <v>5447</v>
+        <v>3263</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="10"/>
-        <v>16928</v>
+        <v>14423</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event11" :{ "type" : "DISASTER", "event_range" : 2252.5284548258, "safe_range" : 4505.05690965161, "max_range" : 6757.58536447741, "intensity" : 8, "start" : 6269, "end" : 11669, "location" : { "x" : 5447, "y" : 16928} },</v>
+        <v>"event11" :{ "type" : "DISASTER", "event_range" : 217.969489048573, "safe_range" : 435.938978097145, "max_range" : 653.908467145718, "intensity" : 5, "start" : 481, "end" : 4210, "location" : { "x" : 3263, "y" : 14423} },</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1172,43 +1172,43 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="2"/>
-        <v>266.31532961920425</v>
+        <v>396.72701272978156</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="3"/>
-        <v>532.6306592384085</v>
+        <v>793.45402545956313</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="4"/>
-        <v>798.94598885761275</v>
+        <v>1190.1810381893447</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="6"/>
-        <v>16554</v>
+        <v>3447</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="7"/>
-        <v>5353</v>
+        <v>5892</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="8"/>
-        <v>21907</v>
+        <v>9339</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="9"/>
-        <v>11439</v>
+        <v>12009</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="10"/>
-        <v>8804</v>
+        <v>14632</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event12" :{ "type" : "DISASTER", "event_range" : 266.315329619204, "safe_range" : 532.630659238408, "max_range" : 798.945988857613, "intensity" : 1, "start" : 16554, "end" : 21907, "location" : { "x" : 11439, "y" : 8804} },</v>
+        <v>"event12" :{ "type" : "DISASTER", "event_range" : 396.727012729782, "safe_range" : 793.454025459563, "max_range" : 1190.18103818934, "intensity" : 2, "start" : 3447, "end" : 9339, "location" : { "x" : 12009, "y" : 14632} },</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1220,15 +1220,15 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="2"/>
-        <v>717.81028048813937</v>
+        <v>2183.3696152356292</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="3"/>
-        <v>1435.6205609762787</v>
+        <v>4366.7392304712585</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="4"/>
-        <v>2153.4308414644183</v>
+        <v>6550.1088457068872</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="5"/>
@@ -1236,27 +1236,27 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="6"/>
-        <v>19467</v>
+        <v>17086</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="7"/>
-        <v>5202</v>
+        <v>4352</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="8"/>
-        <v>24669</v>
+        <v>21438</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="9"/>
-        <v>13681</v>
+        <v>7617</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="10"/>
-        <v>15790</v>
+        <v>16792</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event13" :{ "type" : "DISASTER", "event_range" : 717.810280488139, "safe_range" : 1435.62056097628, "max_range" : 2153.43084146442, "intensity" : 9, "start" : 19467, "end" : 24669, "location" : { "x" : 13681, "y" : 15790} },</v>
+        <v>"event13" :{ "type" : "DISASTER", "event_range" : 2183.36961523563, "safe_range" : 4366.73923047126, "max_range" : 6550.10884570689, "intensity" : 9, "start" : 17086, "end" : 21438, "location" : { "x" : 7617, "y" : 16792} },</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1268,43 +1268,43 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="2"/>
-        <v>202.06882537468653</v>
+        <v>805.79456138706576</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="3"/>
-        <v>404.13765074937305</v>
+        <v>1611.5891227741315</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="4"/>
-        <v>606.20647612405958</v>
+        <v>2417.3836841611974</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="6"/>
-        <v>4772</v>
+        <v>18101</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="7"/>
-        <v>2610</v>
+        <v>5870</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="8"/>
-        <v>7382</v>
+        <v>23971</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="9"/>
-        <v>12929</v>
+        <v>11150</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="10"/>
-        <v>15329</v>
+        <v>193</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event14" :{ "type" : "DISASTER", "event_range" : 202.068825374687, "safe_range" : 404.137650749373, "max_range" : 606.20647612406, "intensity" : 4, "start" : 4772, "end" : 7382, "location" : { "x" : 12929, "y" : 15329} },</v>
+        <v>"event14" :{ "type" : "DISASTER", "event_range" : 805.794561387066, "safe_range" : 1611.58912277413, "max_range" : 2417.3836841612, "intensity" : 3, "start" : 18101, "end" : 23971, "location" : { "x" : 11150, "y" : 193} },</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1316,15 +1316,15 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="2"/>
-        <v>469.16188687167823</v>
+        <v>875.4870142792754</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="3"/>
-        <v>938.32377374335647</v>
+        <v>1750.9740285585508</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="4"/>
-        <v>1407.4856606150347</v>
+        <v>2626.4610428378264</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="5"/>
@@ -1332,27 +1332,27 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="6"/>
-        <v>6033</v>
+        <v>8992</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="7"/>
-        <v>2611</v>
+        <v>2738</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="8"/>
-        <v>8644</v>
+        <v>11730</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="9"/>
-        <v>19937</v>
+        <v>1290</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="10"/>
-        <v>10045</v>
+        <v>19170</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event15" :{ "type" : "DISASTER", "event_range" : 469.161886871678, "safe_range" : 938.323773743356, "max_range" : 1407.48566061503, "intensity" : 10, "start" : 6033, "end" : 8644, "location" : { "x" : 19937, "y" : 10045} },</v>
+        <v>"event15" :{ "type" : "DISASTER", "event_range" : 875.487014279275, "safe_range" : 1750.97402855855, "max_range" : 2626.46104283783, "intensity" : 10, "start" : 8992, "end" : 11730, "location" : { "x" : 1290, "y" : 19170} },</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1364,43 +1364,43 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="2"/>
-        <v>1204.0297562938065</v>
+        <v>783.51177617195697</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="3"/>
-        <v>2408.059512587613</v>
+        <v>1567.0235523439139</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="4"/>
-        <v>3612.0892688814192</v>
+        <v>2350.5353285158708</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="6"/>
-        <v>7225</v>
+        <v>5463</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="7"/>
-        <v>2068</v>
+        <v>2153</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="8"/>
-        <v>9293</v>
+        <v>7616</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="9"/>
-        <v>11652</v>
+        <v>21593</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="10"/>
-        <v>13493</v>
+        <v>15388</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event16" :{ "type" : "DISASTER", "event_range" : 1204.02975629381, "safe_range" : 2408.05951258761, "max_range" : 3612.08926888142, "intensity" : 6, "start" : 7225, "end" : 9293, "location" : { "x" : 11652, "y" : 13493} },</v>
+        <v>"event16" :{ "type" : "DISASTER", "event_range" : 783.511776171957, "safe_range" : 1567.02355234391, "max_range" : 2350.53532851587, "intensity" : 10, "start" : 5463, "end" : 7616, "location" : { "x" : 21593, "y" : 15388} },</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1412,43 +1412,43 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="2"/>
-        <v>601.03672248573662</v>
+        <v>400.34024957908366</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="3"/>
-        <v>1202.0734449714732</v>
+        <v>800.68049915816732</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="4"/>
-        <v>1803.1101674572099</v>
+        <v>1201.0207487372509</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="6"/>
-        <v>4413</v>
+        <v>3751</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="7"/>
-        <v>2695</v>
+        <v>4405</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="8"/>
-        <v>7108</v>
+        <v>8156</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="9"/>
-        <v>21100</v>
+        <v>15735</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="10"/>
-        <v>14927</v>
+        <v>9658</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event17" :{ "type" : "DISASTER", "event_range" : 601.036722485737, "safe_range" : 1202.07344497147, "max_range" : 1803.11016745721, "intensity" : 4, "start" : 4413, "end" : 7108, "location" : { "x" : 21100, "y" : 14927} },</v>
+        <v>"event17" :{ "type" : "DISASTER", "event_range" : 400.340249579084, "safe_range" : 800.680499158167, "max_range" : 1201.02074873725, "intensity" : 3, "start" : 3751, "end" : 8156, "location" : { "x" : 15735, "y" : 9658} },</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1460,43 +1460,43 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="2"/>
-        <v>340.06742970834853</v>
+        <v>132.29995441900115</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="3"/>
-        <v>680.13485941669705</v>
+        <v>264.59990883800231</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="4"/>
-        <v>1020.2022891250456</v>
+        <v>396.89986325700346</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="6"/>
-        <v>17217</v>
+        <v>5686</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="7"/>
-        <v>3068</v>
+        <v>4811</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="8"/>
-        <v>20285</v>
+        <v>10497</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="9"/>
-        <v>10910</v>
+        <v>7920</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="10"/>
-        <v>4409</v>
+        <v>12261</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event18" :{ "type" : "DISASTER", "event_range" : 340.067429708349, "safe_range" : 680.134859416697, "max_range" : 1020.20228912505, "intensity" : 3, "start" : 17217, "end" : 20285, "location" : { "x" : 10910, "y" : 4409} },</v>
+        <v>"event18" :{ "type" : "DISASTER", "event_range" : 132.299954419001, "safe_range" : 264.599908838002, "max_range" : 396.899863257003, "intensity" : 7, "start" : 5686, "end" : 10497, "location" : { "x" : 7920, "y" : 12261} },</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1508,43 +1508,43 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="2"/>
-        <v>227.54643708175388</v>
+        <v>1558.8727273327424</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="3"/>
-        <v>455.09287416350776</v>
+        <v>3117.7454546654849</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="4"/>
-        <v>682.63931124526164</v>
+        <v>4676.6181819982276</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="6"/>
-        <v>12179</v>
+        <v>4746</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="7"/>
-        <v>4846</v>
+        <v>2655</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="8"/>
-        <v>17025</v>
+        <v>7401</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="9"/>
-        <v>5367</v>
+        <v>14809</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="10"/>
-        <v>7293</v>
+        <v>18785</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>"event19" :{ "type" : "DISASTER", "event_range" : 227.546437081754, "safe_range" : 455.092874163508, "max_range" : 682.639311245262, "intensity" : 2, "start" : 12179, "end" : 17025, "location" : { "x" : 5367, "y" : 7293} },</v>
+        <v>"event19" :{ "type" : "DISASTER", "event_range" : 1558.87272733274, "safe_range" : 3117.74545466548, "max_range" : 4676.61818199823, "intensity" : 6, "start" : 4746, "end" : 7401, "location" : { "x" : 14809, "y" : 18785} },</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1556,43 +1556,43 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="2"/>
-        <v>276.38597663590355</v>
+        <v>114.75794614676434</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="3"/>
-        <v>552.77195327180709</v>
+        <v>229.51589229352868</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="4"/>
-        <v>829.1579299077107</v>
+        <v>344.27383844029305</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="6"/>
-        <v>4104</v>
+        <v>16130</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="7"/>
-        <v>3738</v>
+        <v>2463</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="8"/>
-        <v>7842</v>
+        <v>18593</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="9"/>
-        <v>5997</v>
+        <v>13520</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="10"/>
-        <v>14536</v>
+        <v>12912</v>
       </c>
       <c r="N25" t="str">
         <f ca="1">CONCATENATE("""",A25,""" :{ ""type"" : """,B25,""", ""event_range"" : ",C25,", ""safe_range"" : ",D25,", ""max_range"" : ",E25,", ""intensity"" : ",F25,", ""start"" : ",G25,", ""end"" : ",I25,", ""location"" : { ""x"" : ",J25,", ""y"" : ",K25,"} }")</f>
-        <v>"event20" :{ "type" : "DISASTER", "event_range" : 276.385976635904, "safe_range" : 552.771953271807, "max_range" : 829.157929907711, "intensity" : 3, "start" : 4104, "end" : 7842, "location" : { "x" : 5997, "y" : 14536} }</v>
+        <v>"event20" :{ "type" : "DISASTER", "event_range" : 114.757946146764, "safe_range" : 229.515892293529, "max_range" : 344.273838440293, "intensity" : 6, "start" : 16130, "end" : 18593, "location" : { "x" : 13520, "y" : 12912} }</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>